<commit_message>
Feat: Refatoração de fucnionários e horas
</commit_message>
<xml_diff>
--- a/Relatorio_Alocacao_2025-07-10.xlsx
+++ b/Relatorio_Alocacao_2025-07-10.xlsx
@@ -221,7 +221,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Consolidado'!K2</f>
+              <f>'Consolidado'!J2</f>
             </strRef>
           </tx>
           <spPr>
@@ -237,12 +237,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Consolidado'!$J$3:$J$5</f>
+              <f>'Consolidado'!$I$3:$I$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Consolidado'!$K$3:$K$5</f>
+              <f>'Consolidado'!$J$3:$J$4</f>
             </numRef>
           </val>
         </ser>
@@ -356,7 +356,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Lote 1'!K2</f>
+              <f>'Lote 1'!J2</f>
             </strRef>
           </tx>
           <spPr>
@@ -372,12 +372,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Lote 1'!$J$3:$J$5</f>
+              <f>'Lote 1'!$I$3:$I$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Lote 1'!$K$3:$K$5</f>
+              <f>'Lote 1'!$J$3:$J$4</f>
             </numRef>
           </val>
         </ser>
@@ -445,7 +445,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>9</row>
+      <row>10</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -472,7 +472,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>9</row>
+      <row>10</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -782,7 +782,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -790,13 +790,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
     <col width="25" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -827,11 +826,6 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Mar/24</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
           <t>H.mês</t>
         </is>
       </c>
@@ -839,15 +833,15 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Drenagem</t>
+          <t>Coordenação</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Mês</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
-        <is>
-          <t>Mês</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
         <is>
           <t>Total Decimal</t>
         </is>
@@ -856,12 +850,12 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Drenagem</t>
+          <t>Coordenação</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -871,97 +865,135 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>1,04</t>
+          <t>0,38</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>1,04</t>
+          <t>0,38</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>1,04</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>3,12</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
+          <t>0,75</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>Jan/24</t>
         </is>
       </c>
-      <c r="K3" t="n">
-        <v>2.92</v>
+      <c r="J3" t="n">
+        <v>1.52</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Estruturas</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Coordenação</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>teste1</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>0,75</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>Feb/24</t>
         </is>
       </c>
-      <c r="K4" t="n">
-        <v>2.92</v>
+      <c r="J4" t="n">
+        <v>1.52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Estruturas</t>
+          <t>Coordenação</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
+          <t>Eng. Sênior</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>teste2</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>0,75</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Coordenação</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
           <t>Estagiário/Projetista</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>tets1</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>1,88</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>1,88</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>1,88</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="inlineStr">
-        <is>
-          <t>5,62</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Mar/24</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>2.92</v>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>teste3</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>0,75</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -974,7 +1006,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -982,13 +1014,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
     <col width="25" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1019,11 +1050,6 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Mar/24</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
           <t>H.mês</t>
         </is>
       </c>
@@ -1031,15 +1057,15 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Drenagem</t>
+          <t>Coordenação</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Mês</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
-        <is>
-          <t>Mês</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
         <is>
           <t>Total Decimal</t>
         </is>
@@ -1048,12 +1074,12 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Drenagem</t>
+          <t>Coordenação</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -1063,97 +1089,135 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>1,04</t>
+          <t>0,38</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>1,04</t>
+          <t>0,38</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>1,04</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>3,12</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
+          <t>0,75</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>Jan/24</t>
         </is>
       </c>
-      <c r="K3" t="n">
-        <v>2.92</v>
+      <c r="J3" t="n">
+        <v>1.52</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Estruturas</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Coordenação</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>teste1</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>0,75</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>Feb/24</t>
         </is>
       </c>
-      <c r="K4" t="n">
-        <v>2.92</v>
+      <c r="J4" t="n">
+        <v>1.52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Estruturas</t>
+          <t>Coordenação</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
+          <t>Eng. Sênior</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>teste2</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>0,75</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Coordenação</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
           <t>Estagiário/Projetista</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>tets1</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>1,88</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>1,88</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>1,88</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="inlineStr">
-        <is>
-          <t>5,62</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Mar/24</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>2.92</v>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>teste3</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>0,38</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>0,75</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>